<commit_message>
Update PatientData.xlsx with latest test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/PatientData.xlsx
+++ b/src/test/resources/testdata/PatientData.xlsx
@@ -37,16 +37,16 @@
     <t xml:space="preserve">Date of Birth</t>
   </si>
   <si>
-    <t xml:space="preserve">Tim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tim@d.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04/03/2000</t>
+    <t xml:space="preserve">Phil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phil@s.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/27/1989</t>
   </si>
 </sst>
 </file>
@@ -291,7 +291,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -330,7 +330,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>8392394039</v>
+        <v>3328293043</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>8</v>
@@ -338,7 +338,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Tim@d.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="phil@s.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>